<commit_message>
Objets Chambre d'Abi Intégration + Ecriture Objets Chambre d'Hippo
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/TABLE_REFERENCE_LOCALISATION2.xlsx
+++ b/Assets/StreamingAssets/TABLE_REFERENCE_LOCALISATION2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" tabRatio="817" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" tabRatio="817" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Act1Niv0" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="Salon" sheetId="10" r:id="rId10"/>
     <sheet name="ChambreAbi" sheetId="11" r:id="rId11"/>
     <sheet name="ChambreHip" sheetId="12" r:id="rId12"/>
-    <sheet name="ChambreCel" sheetId="13" r:id="rId13"/>
-    <sheet name="Jardin" sheetId="14" r:id="rId14"/>
+    <sheet name="Jardin" sheetId="14" r:id="rId13"/>
+    <sheet name="ChambreCel" sheetId="13" r:id="rId14"/>
     <sheet name="Grenier" sheetId="15" r:id="rId15"/>
   </sheets>
   <definedNames>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14786" uniqueCount="5754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14998" uniqueCount="5821">
   <si>
     <t>LINE</t>
   </si>
@@ -17241,9 +17241,6 @@
     <t>It's Abigail's rocking elephant. It's her favorite animal.</t>
   </si>
   <si>
-    <t>ChambreAbi</t>
-  </si>
-  <si>
     <t>Lamp</t>
   </si>
   <si>
@@ -17289,12 +17286,6 @@
     <t>DeskPicture</t>
   </si>
   <si>
-    <t>DeskChair</t>
-  </si>
-  <si>
-    <t>DeskLamp</t>
-  </si>
-  <si>
     <t>PARCHEESI</t>
   </si>
   <si>
@@ -17302,13 +17293,223 @@
   </si>
   <si>
     <t>Drawers</t>
+  </si>
+  <si>
+    <t>Abigail a des tonnes de souvenirs ici. Elle affiche tout, on voit des photos de tout le monde a tous les âges.</t>
+  </si>
+  <si>
+    <t>Abigail has so many memories in this place. She keeps everything. She has pictures of everyone throughout her life.</t>
+  </si>
+  <si>
+    <t>Je ne vais pas fouiller dans les affaires personnelles d'Abigail.</t>
+  </si>
+  <si>
+    <t>Je me demande ce qu'Abigail range là-dedans.</t>
+  </si>
+  <si>
+    <t>Les plantes m'apaisent. Elles sont en bonne santé, aucune n'a besoin d'être arrosée.</t>
+  </si>
+  <si>
+    <t>Je n'ai jamais eu de coiffeuse. Quand je pense qu'elle a aussi une salle de bain personnelle…</t>
+  </si>
+  <si>
+    <t>Les fenêtres donnent sur le jardin. La vue est magnifique.</t>
+  </si>
+  <si>
+    <t>Je n'ai pas envie de m'asseoir maintenant.</t>
+  </si>
+  <si>
+    <t>Les tapis sont tout doux sous mes pieds.</t>
+  </si>
+  <si>
+    <t>Encore une photo de famille.</t>
+  </si>
+  <si>
+    <t>C'est ici qu'Abigail doit s'installer pour écrire.</t>
+  </si>
+  <si>
+    <t>Je n'ai pas besoin de plus de lumière.</t>
+  </si>
+  <si>
+    <t>C'est la première fois que je vois un banc de lit dans la vraie vie.</t>
+  </si>
+  <si>
+    <t>Oh, des lapins ! Dommage que ça ne soient que des statuettes.</t>
+  </si>
+  <si>
+    <t>I don't want to go through Abigail's personal stuff.</t>
+  </si>
+  <si>
+    <t>I don't need more light.</t>
+  </si>
+  <si>
+    <t>A canopy bed! What a dream!</t>
+  </si>
+  <si>
+    <t>Un lit à baldaquin ! Un rêve éveillé…</t>
+  </si>
+  <si>
+    <t>Abigail reads so much. I can't even start to count the number of classic novels she has in her room, let alone in the library.</t>
+  </si>
+  <si>
+    <t>Abigail lit énormément. Elle a un nombre incalculable de classiques… Et encore, ce ne sont que ceux qu'elle garde dans sa chambre. Elle doit en avoir encore beaucoup dans la bibliothèque.</t>
+  </si>
+  <si>
+    <t>I wonder what Abigail keeps in here.</t>
+  </si>
+  <si>
+    <t>Oh, rabbits! Too bad they're fake.</t>
+  </si>
+  <si>
+    <t>The plants comfort me. They're all healthy. None of them need watering.</t>
+  </si>
+  <si>
+    <t>I've never had a dressing table. And Abigail also has her own private bathroom...</t>
+  </si>
+  <si>
+    <t>The view on the garden is beautiful.</t>
+  </si>
+  <si>
+    <t>I don't want to sit right now.</t>
+  </si>
+  <si>
+    <t>The carpets are so soft under my feet.</t>
+  </si>
+  <si>
+    <t>Another family portrait.</t>
+  </si>
+  <si>
+    <t>It's the first time I see a bedside bench in real life.</t>
+  </si>
+  <si>
+    <t>That's where Abigail must sit to write.</t>
+  </si>
+  <si>
+    <t>CHAMBREHIPPO</t>
+  </si>
+  <si>
+    <t>COMPUTER</t>
+  </si>
+  <si>
+    <t>SPEAKERS</t>
+  </si>
+  <si>
+    <t>CHAIR</t>
+  </si>
+  <si>
+    <t>CAMERA</t>
+  </si>
+  <si>
+    <t>SHOES</t>
+  </si>
+  <si>
+    <t>BED</t>
+  </si>
+  <si>
+    <t>GUITAR</t>
+  </si>
+  <si>
+    <t>SHIRT</t>
+  </si>
+  <si>
+    <t>HIDDEN_TRAP</t>
+  </si>
+  <si>
+    <t>CDS</t>
+  </si>
+  <si>
+    <t>CLARINET</t>
+  </si>
+  <si>
+    <t>HEAD_OF_BED</t>
+  </si>
+  <si>
+    <t>PAPERS_ON_FLOOR</t>
+  </si>
+  <si>
+    <t>BOTTLES</t>
+  </si>
+  <si>
+    <t>BEDSIDE_BOOKS</t>
+  </si>
+  <si>
+    <t>HEADPHONES</t>
+  </si>
+  <si>
+    <t>Abigailsroom</t>
+  </si>
+  <si>
+    <t>Pictures Inventaire</t>
+  </si>
+  <si>
+    <t>Abigail a des tonnes de souvenirs au Manoir. Elle prend tout en photo.</t>
+  </si>
+  <si>
+    <t>Abigail has so many memories of the Manor. She took pictures of everything.</t>
+  </si>
+  <si>
+    <t>Hippolyte peint vraiment énormément ! Sa chambre est tellement personnelle, je ne m'y attendais pas du tout.</t>
+  </si>
+  <si>
+    <t>Un ordinateur dernier cri… La session est bloquée par un mot de passe, je ne peux pas y accéder.</t>
+  </si>
+  <si>
+    <t>Hippolyte a tout ce qu'il faut pour pouvoir écouter de la musique dans de bonnes conditions.</t>
+  </si>
+  <si>
+    <t>Même si je voulais m'asseoir, je ne pourrais pas, cette chaise sert visiblement à y poser les choses qui ne sont pas par terre.</t>
+  </si>
+  <si>
+    <t>Un appareil photo ? Hippolyte fait beaucoup plus d'activités artistiques que je ne le croyais.</t>
+  </si>
+  <si>
+    <t>Il faut que je fasse attention de ne pas trébucher, il y a des affaires un peu partout.</t>
+  </si>
+  <si>
+    <t>Le lit est défait, comme une invitation à revenir s'y prélasser.</t>
+  </si>
+  <si>
+    <t>Je ne savais pas qu'Hippolyte jouait de la guitare.</t>
+  </si>
+  <si>
+    <t>Une clarinette ! Je trouve que ça colle bien à sa personnalité.</t>
+  </si>
+  <si>
+    <t>On dirait des brouillons de composition. Il écrit donc de la musique ?</t>
+  </si>
+  <si>
+    <t>Tiens… Qu'est-ce que c'est ? Un recoin secret ? Qu'est-ce qu'Hippolyte peut bien vouloir cacher ?</t>
+  </si>
+  <si>
+    <t>C'est du matériel de tatouage. Les aiguilles, l'encre, et même un carnet avec des designs… Est-ce que c'est Hippolyte qui les a fait ? J'ai l'impression de reconnaître son style, et en même temps c'est tellement différent de ce qui est accroché sur les murs...</t>
+  </si>
+  <si>
+    <t>L'ampoule a grillé.</t>
+  </si>
+  <si>
+    <t>C'est de l'eau. Je crois.</t>
+  </si>
+  <si>
+    <t>Encore de quoi écouter de la musique. Hippolyte a l'air de souvent s'isoler dans sa bulle de sons.</t>
+  </si>
+  <si>
+    <t>Ces boîtes sont trop hautes pour que je les attrape sans monter debout sur le lit. Je n'en ai pas envie.</t>
+  </si>
+  <si>
+    <t>Dernières lectures : Châteaux de la colère, La Maison dans Laquelle et Emma Goldman : Epopée d'une Anarchiste.</t>
+  </si>
+  <si>
+    <t>Je ne vois rien de spécial…</t>
+  </si>
+  <si>
+    <t>Ce sont surtout des carnets à croquis et quelques livres théoriques sur l'Histoire de l'Art.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -17344,6 +17545,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -17409,7 +17617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -17448,6 +17656,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20368,305 +20580,568 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" customWidth="1"/>
-    <col min="7" max="7" width="52.85546875" customWidth="1"/>
-    <col min="8" max="28" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="39" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="29" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5604</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4689</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="B2" t="s">
+      <c r="I1" s="17" t="s">
+        <v>5609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1">
+      <c r="A2" t="str">
+        <f>CONCATENATE(D2,"_",MID(C2,1,3),"_",MID(F2,1,3),"_",MID(E2,1,3),"_",B2)</f>
+        <v>A01_Abi_NAR_Dra_00010</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5605</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5750</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4694</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>5753</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>5765</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A18" si="0">CONCATENATE(D3,"_",MID(C3,1,3),"_",MID(F3,1,3),"_",MID(E3,1,3),"_",B3)</f>
+        <v>A01_Abi_NAR_Lam_00020</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5605</v>
+      </c>
+      <c r="E3" t="s">
         <v>5733</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F3" t="s">
+        <v>4694</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>5762</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>5766</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Bed_00030</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D4" t="s">
         <v>5605</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E4" t="s">
+        <v>5734</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4694</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>5768</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>5767</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Boo_00040</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5605</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5735</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4694</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>5770</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>5769</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Che_00050</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5605</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5736</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4694</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>5754</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>5771</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Rab_00060</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5605</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5737</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4694</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>5764</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>5772</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Cup_00070</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5605</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5738</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4694</v>
+      </c>
+      <c r="G8" t="s">
         <v>5753</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H8" s="17" t="s">
+        <v>5765</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Pla_00080</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5605</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5739</v>
+      </c>
+      <c r="F9" t="s">
         <v>4694</v>
       </c>
-      <c r="H2" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
-      <c r="B3" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="G9" s="17" t="s">
+        <v>5755</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>5773</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Mir_00090</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D10" t="s">
         <v>5605</v>
       </c>
-      <c r="D3" t="s">
-        <v>5734</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E10" t="s">
+        <v>5740</v>
+      </c>
+      <c r="F10" t="s">
         <v>4694</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="B4" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G10" s="17" t="s">
+        <v>5756</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>5774</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Win_00100</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D11" t="s">
         <v>5605</v>
       </c>
-      <c r="D4" t="s">
-        <v>5735</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E11" t="s">
+        <v>5741</v>
+      </c>
+      <c r="F11" t="s">
         <v>4694</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="B5" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="G11" s="17" t="s">
+        <v>5757</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>5775</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Cha_00110</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D12" t="s">
         <v>5605</v>
       </c>
-      <c r="D5" t="s">
-        <v>5736</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E12" t="s">
+        <v>5743</v>
+      </c>
+      <c r="F12" t="s">
         <v>4694</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="B6" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="G12" s="17" t="s">
+        <v>5758</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>5776</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Pic_00120</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D13" t="s">
         <v>5605</v>
       </c>
-      <c r="D6" t="s">
-        <v>5737</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="E13" s="29" t="s">
+        <v>5744</v>
+      </c>
+      <c r="F13" t="s">
         <v>4694</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
-      <c r="B7" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="G13" s="30" t="s">
+        <v>5751</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>5752</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Car_00130</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D14" t="s">
         <v>5605</v>
       </c>
-      <c r="D7" t="s">
-        <v>5738</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="E14" t="s">
+        <v>5742</v>
+      </c>
+      <c r="F14" t="s">
         <v>4694</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
-      <c r="B8" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="G14" s="17" t="s">
+        <v>5759</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>5777</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Des_00140</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D15" t="s">
         <v>5605</v>
       </c>
-      <c r="D8" t="s">
-        <v>5739</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E15" t="s">
+        <v>5747</v>
+      </c>
+      <c r="F15" t="s">
         <v>4694</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
-      <c r="B9" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="G15" s="17" t="s">
+        <v>5760</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>5778</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Bed_00150</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D16" t="s">
         <v>5605</v>
       </c>
-      <c r="D9" t="s">
-        <v>5740</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="E16" t="s">
+        <v>5746</v>
+      </c>
+      <c r="F16" t="s">
         <v>4694</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
-      <c r="B10" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="G16" s="17" t="s">
+        <v>5763</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>5779</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Pap_00160</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>5605</v>
       </c>
-      <c r="D10" t="s">
-        <v>5741</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="E17" t="s">
+        <v>5745</v>
+      </c>
+      <c r="F17" t="s">
         <v>4694</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
-      <c r="B11" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="G17" s="17" t="s">
+        <v>5761</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>5780</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_Abi_NAR_Pic_00170</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>5798</v>
+      </c>
+      <c r="D18" t="s">
         <v>5605</v>
       </c>
-      <c r="D11" t="s">
-        <v>5742</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="E18" s="31" t="s">
+        <v>5799</v>
+      </c>
+      <c r="F18" t="s">
         <v>4694</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
-      <c r="B12" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5605</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5744</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4694</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1">
-      <c r="B13" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5605</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>5745</v>
-      </c>
-      <c r="E13" t="s">
-        <v>4694</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
-      <c r="B14" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5605</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5743</v>
-      </c>
-      <c r="E14" t="s">
-        <v>4694</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="B15" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5605</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5748</v>
-      </c>
-      <c r="E15" t="s">
-        <v>4694</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="B16" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5605</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5749</v>
-      </c>
-      <c r="E16" t="s">
-        <v>4694</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="15" customHeight="1">
-      <c r="B17" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5605</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5750</v>
-      </c>
-      <c r="E17" t="s">
-        <v>4694</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="15" customHeight="1">
-      <c r="B18" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5605</v>
-      </c>
-      <c r="D18" t="s">
-        <v>5746</v>
-      </c>
-      <c r="E18" t="s">
-        <v>4694</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="15" customHeight="1">
-      <c r="B19" t="s">
-        <v>5733</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5605</v>
-      </c>
-      <c r="D19" t="s">
-        <v>5747</v>
-      </c>
-      <c r="E19" t="s">
-        <v>4694</v>
+      <c r="G18" s="17" t="s">
+        <v>5800</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>5801</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>5610</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -20675,32 +21150,484 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="35.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="28" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="17" t="s">
+        <v>5604</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>4689</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>5609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1">
+      <c r="B2" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>4833</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>5802</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1">
+      <c r="B3" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>5782</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>5803</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1">
+      <c r="B4" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>5783</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>5804</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1">
+      <c r="B5" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>5784</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>5805</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1">
+      <c r="B6" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>5785</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>5806</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1">
+      <c r="B7" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>5132</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>5820</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1">
+      <c r="B8" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>5786</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>5807</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1">
+      <c r="B9" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>5787</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>5808</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1">
+      <c r="B10" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>5788</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>5809</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1">
+      <c r="B11" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>5789</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>5819</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1">
+      <c r="B12" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>5790</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>5812</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1">
+      <c r="B13" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>5790</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1">
+      <c r="B14" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>5790</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>5813</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1">
+      <c r="B15" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>5791</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1">
+      <c r="B16" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>5792</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>5810</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1">
+      <c r="B17" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>4711</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>5814</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15" customHeight="1">
+      <c r="B18" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>5793</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15" customHeight="1">
+      <c r="B19" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>5794</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>5811</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15" customHeight="1">
+      <c r="B20" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>5795</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>5815</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="15" customHeight="1">
+      <c r="B21" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>5796</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>5818</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15" customHeight="1">
+      <c r="B22" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>5797</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>5816</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>5611</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="15" customHeight="1">
+      <c r="B23" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>5120</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>5817</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>5611</v>
       </c>
     </row>
   </sheetData>
@@ -20714,30 +21641,98 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="10.7109375" customWidth="1"/>
+    <col min="1" max="28" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="17" t="s">
+        <v>5604</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>4689</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1">
+      <c r="C2" s="17" t="s">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1">
+      <c r="C3" s="17" t="s">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1">
+      <c r="C4" s="17" t="s">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1">
+      <c r="C5" s="17" t="s">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1">
+      <c r="C6" s="17" t="s">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1">
+      <c r="C7" s="17" t="s">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1">
+      <c r="C8" s="17" t="s">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1">
+      <c r="C9" s="17" t="s">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1">
+      <c r="C10" s="17" t="s">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1">
+      <c r="C11" s="17" t="s">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1">
+      <c r="C12" s="17" t="s">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1">
+      <c r="C13" s="17" t="s">
+        <v>5605</v>
       </c>
     </row>
   </sheetData>
@@ -20827,7 +21822,7 @@
   </sheetPr>
   <dimension ref="A1:H312"/>
   <sheetViews>
-    <sheetView topLeftCell="A295" workbookViewId="0">
+    <sheetView topLeftCell="A292" workbookViewId="0">
       <selection activeCell="A280" sqref="A280"/>
     </sheetView>
   </sheetViews>
@@ -62809,7 +63804,7 @@
   </sheetPr>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
@@ -64599,7 +65594,7 @@
   </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -65376,8 +66371,8 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -65628,7 +66623,7 @@
         <v>5696</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>5752</v>
+        <v>5749</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -66126,7 +67121,7 @@
         <v>5605</v>
       </c>
       <c r="E25" t="s">
-        <v>5751</v>
+        <v>5748</v>
       </c>
       <c r="F25" t="s">
         <v>4694</v>

</xml_diff>

<commit_message>
Localisation + Intégration Objets Chambre Hippolyte
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/TABLE_REFERENCE_LOCALISATION2.xlsx
+++ b/Assets/StreamingAssets/TABLE_REFERENCE_LOCALISATION2.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14998" uniqueCount="5821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15053" uniqueCount="5847">
   <si>
     <t>LINE</t>
   </si>
@@ -17503,6 +17503,84 @@
   </si>
   <si>
     <t>Ce sont surtout des carnets à croquis et quelques livres théoriques sur l'Histoire de l'Art.</t>
+  </si>
+  <si>
+    <t>Il y a des CD de métal cachés sous du rock et de la pop.</t>
+  </si>
+  <si>
+    <t>J'aime bien la décoration de la chambre d'Hippolyte, elle est chaleureuse et reposante.</t>
+  </si>
+  <si>
+    <t>00131</t>
+  </si>
+  <si>
+    <t>Hippolyte cache du matériel de tatouage dans un recoin secret dans sa chambre.</t>
+  </si>
+  <si>
+    <t>Hippolyte really paints a lot! His room is so well decorated! I didn't expect that.</t>
+  </si>
+  <si>
+    <t>A high-tech computer… I don't know the password so I can't use it.</t>
+  </si>
+  <si>
+    <t>Hippolyte has everything he needs to listen to music in the best possible way.</t>
+  </si>
+  <si>
+    <t>Even if I wanted to sit down, I couldn't. This chair's purpose is obviously to serve as a table for the things that aren't on the floor.</t>
+  </si>
+  <si>
+    <t>Is that a camera? Hippolyte has so many artistic interests.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These are mostly sketchbooks and manuals about the History of Arts. </t>
+  </si>
+  <si>
+    <t>I need to be careful not to trip. There are stuff everywhere on the floor.</t>
+  </si>
+  <si>
+    <t>The bed isn't made. I feel like it's welcoming me to go back to sleep.</t>
+  </si>
+  <si>
+    <t>I didn't know Hippolyte played the guitar.</t>
+  </si>
+  <si>
+    <t>I don't see anything of interest here…</t>
+  </si>
+  <si>
+    <t>What's that? Is it a secret hideout? What could Hippolyte possibly want to hide?</t>
+  </si>
+  <si>
+    <t>Hippolyte hides everything he needs to tattoo someone in a hideout in his room.</t>
+  </si>
+  <si>
+    <t>It's tattooing gear. There are needles, inks, and even a sketchbook full of designs. Did Hippolyte draw them? I feel like I can recognize his style, but at the same time, it is so different from what's hanging on the walls…</t>
+  </si>
+  <si>
+    <t>There are CDs of metal bands hidden under rock and pop music.</t>
+  </si>
+  <si>
+    <t>A clarinet! That fits with his personality.</t>
+  </si>
+  <si>
+    <t>The lightbulb burned out.</t>
+  </si>
+  <si>
+    <t>I like how Hippolyte's room feels to me. It is confy and warm.</t>
+  </si>
+  <si>
+    <t>This looks like rough drafts of sheet music… Is Hippolyte also a composer?</t>
+  </si>
+  <si>
+    <t>That's water. I think.</t>
+  </si>
+  <si>
+    <t>Last books read: Lands of Glass, The Gray House and Emma Goldman: Living my Life.</t>
+  </si>
+  <si>
+    <t>More equipment to listen to music. Apparently, Hippolyte often isolates himself in a sound bubble.</t>
+  </si>
+  <si>
+    <t>These boxes are too high up for me to reach them without standing on the bed. I don't feel like it.</t>
   </si>
 </sst>
 </file>
@@ -17547,7 +17625,6 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -17656,10 +17733,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+      <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20583,7 +20660,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -20979,7 +21056,7 @@
       <c r="F13" t="s">
         <v>4694</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="31" t="s">
         <v>5751</v>
       </c>
       <c r="H13" s="17" t="s">
@@ -21123,7 +21200,7 @@
       <c r="D18" t="s">
         <v>5605</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="30" t="s">
         <v>5799</v>
       </c>
       <c r="F18" t="s">
@@ -21150,484 +21227,743 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="35.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="28" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="29" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>5604</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>4689</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>5609</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="1:9" ht="15" customHeight="1">
+      <c r="A2" t="str">
+        <f>CONCATENATE(D2,"_",MID(C2,1,3),"_",MID(F2,1,3),"_",MID(E2,1,3),"_",B2)</f>
+        <v>A01_CHA_NAR_ART_00010</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5605</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
         <v>4833</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>5802</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
-      <c r="B3" s="17" t="s">
+      <c r="H2" s="17" t="s">
+        <v>5825</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A24" si="0">CONCATENATE(D3,"_",MID(C3,1,3),"_",MID(F3,1,3),"_",MID(E3,1,3),"_",B3)</f>
+        <v>A01_CHA_NAR_COM_00020</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>5605</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>5782</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>5803</v>
       </c>
-      <c r="H3" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="B4" s="17" t="s">
+      <c r="H3" s="17" t="s">
+        <v>5826</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_SPE_00030</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>5605</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>5783</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>5804</v>
       </c>
-      <c r="H4" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="B5" s="17" t="s">
+      <c r="H4" s="17" t="s">
+        <v>5827</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_CHA_00040</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>5605</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>5784</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="17" t="s">
         <v>5805</v>
       </c>
-      <c r="H5" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="B6" s="17" t="s">
+      <c r="H5" s="17" t="s">
+        <v>5828</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_CAM_00050</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>5605</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="E6" s="17" t="s">
         <v>5785</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="F6" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="G6" s="17" t="s">
         <v>5806</v>
       </c>
-      <c r="H6" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
-      <c r="B7" s="17" t="s">
+      <c r="H6" s="17" t="s">
+        <v>5829</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_BOO_00060</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>5605</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E7" s="17" t="s">
         <v>5132</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="F7" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="G7" s="17" t="s">
         <v>5820</v>
       </c>
-      <c r="H7" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
-      <c r="B8" s="17" t="s">
+      <c r="H7" s="17" t="s">
+        <v>5830</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_SHO_00070</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>5605</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="E8" s="17" t="s">
         <v>5786</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="F8" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="17" t="s">
         <v>5807</v>
       </c>
-      <c r="H8" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
-      <c r="B9" s="17" t="s">
+      <c r="H8" s="17" t="s">
+        <v>5831</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_BED_00080</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>5605</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="E9" s="17" t="s">
         <v>5787</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="F9" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>5808</v>
       </c>
-      <c r="H9" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
-      <c r="B10" s="17" t="s">
+      <c r="H9" s="17" t="s">
+        <v>5832</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_GUI_00090</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>5605</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="E10" s="17" t="s">
         <v>5788</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="F10" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="G10" s="17" t="s">
         <v>5809</v>
       </c>
-      <c r="H10" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
-      <c r="B11" s="17" t="s">
+      <c r="H10" s="17" t="s">
+        <v>5833</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_SHI_00100</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>5605</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="17" t="s">
         <v>5789</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="F11" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="G11" s="17" t="s">
         <v>5819</v>
       </c>
-      <c r="H11" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
-      <c r="B12" s="17" t="s">
+      <c r="H11" s="17" t="s">
+        <v>5834</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_HID_00110</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>5605</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="E12" s="30" t="s">
         <v>5790</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="F12" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="G12" s="17" t="s">
         <v>5812</v>
       </c>
-      <c r="H12" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1">
-      <c r="B13" s="17" t="s">
+      <c r="H12" s="17" t="s">
+        <v>5835</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_HID_00120</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="D13" s="17" t="s">
         <v>5605</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="E13" s="30" t="s">
         <v>5790</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="F13" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="G13" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="H13" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
-      <c r="B14" s="17" t="s">
+      <c r="H13" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_HID_00131</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>5823</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="D14" s="17" t="s">
         <v>5605</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="E14" s="30" t="s">
         <v>5790</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="F14" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="G14" s="17" t="s">
+        <v>5824</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>5836</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_HID_00130</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>5781</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>5605</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>5790</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="G15" s="17" t="s">
         <v>5813</v>
       </c>
-      <c r="H14" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="B15" s="17" t="s">
+      <c r="H15" s="17" t="s">
+        <v>5837</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_CDS_00140</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D16" t="s">
         <v>5605</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="E16" s="17" t="s">
         <v>5791</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="F16" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="H15" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="B16" s="17" t="s">
+      <c r="G16" s="17" t="s">
+        <v>5821</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>5838</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_CLA_00150</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D17" t="s">
         <v>5605</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="E17" s="17" t="s">
         <v>5792</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="F17" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="G17" s="17" t="s">
         <v>5810</v>
       </c>
-      <c r="H16" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1">
-      <c r="B17" s="17" t="s">
+      <c r="H17" s="17" t="s">
+        <v>5839</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_LAM_00160</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D18" t="s">
         <v>5605</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="E18" s="17" t="s">
         <v>4711</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="F18" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="G18" s="17" t="s">
         <v>5814</v>
       </c>
-      <c r="H17" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="15" customHeight="1">
-      <c r="B18" s="17" t="s">
+      <c r="H18" s="17" t="s">
+        <v>5840</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_HEA_00170</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D19" t="s">
         <v>5605</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="E19" s="17" t="s">
         <v>5793</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="F19" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="H18" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="15" customHeight="1">
-      <c r="B19" s="17" t="s">
+      <c r="G19" s="17" t="s">
+        <v>5822</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>5841</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_PAP_00180</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D20" t="s">
         <v>5605</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="E20" s="17" t="s">
         <v>5794</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="F20" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="G20" s="17" t="s">
         <v>5811</v>
       </c>
-      <c r="H19" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="15" customHeight="1">
-      <c r="B20" s="17" t="s">
+      <c r="H20" s="17" t="s">
+        <v>5842</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_BOT_00190</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D21" t="s">
         <v>5605</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="E21" s="17" t="s">
         <v>5795</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="F21" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="G21" s="17" t="s">
         <v>5815</v>
       </c>
-      <c r="H20" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="15" customHeight="1">
-      <c r="B21" s="17" t="s">
+      <c r="H21" s="17" t="s">
+        <v>5843</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_BED_00200</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D22" t="s">
         <v>5605</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="E22" s="17" t="s">
         <v>5796</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="F22" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="G22" s="17" t="s">
         <v>5818</v>
       </c>
-      <c r="H21" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="15" customHeight="1">
-      <c r="B22" s="17" t="s">
+      <c r="H22" s="17" t="s">
+        <v>5844</v>
+      </c>
+      <c r="I22" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_HEA_00210</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D23" t="s">
         <v>5605</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="E23" s="17" t="s">
         <v>5797</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="F23" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="G23" s="17" t="s">
         <v>5816</v>
       </c>
-      <c r="H22" s="28" t="s">
-        <v>5611</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="15" customHeight="1">
-      <c r="B23" s="17" t="s">
+      <c r="H23" s="17" t="s">
+        <v>5845</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>A01_CHA_NAR_BOX_00220</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>5781</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D24" t="s">
         <v>5605</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="E24" s="17" t="s">
         <v>5120</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="F24" s="17" t="s">
         <v>4694</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="G24" s="17" t="s">
         <v>5817</v>
       </c>
-      <c r="H23" s="28" t="s">
-        <v>5611</v>
+      <c r="H24" s="17" t="s">
+        <v>5846</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>5610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>